<commit_message>
modified:   Environment.py 	modified:   __pycache__/Environment.cpython-312.pyc 	modified:   __pycache__/Sprites.cpython-312.pyc 	modified:   map_1.xlsx 	modified:   map_2.xlsx 	modified:   map_4.xlsx 	modified:   model.py
</commit_message>
<xml_diff>
--- a/map_1.xlsx
+++ b/map_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VS_project\souless\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A0F1EA-ECA3-4A90-840B-4587E6A724A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A2D084-88D4-40C3-9D09-95AB95E18550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -76,12 +76,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -95,12 +89,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -388,8 +381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC12" sqref="AC12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1890,8 +1883,8 @@
       <c r="AB12" s="2">
         <v>0</v>
       </c>
-      <c r="AC12" s="4">
-        <v>4</v>
+      <c r="AC12" s="2">
+        <v>0</v>
       </c>
       <c r="AD12" s="2">
         <v>0</v>
@@ -2640,8 +2633,8 @@
       <c r="V18" s="2">
         <v>0</v>
       </c>
-      <c r="W18" s="4">
-        <v>4</v>
+      <c r="W18" s="2">
+        <v>0</v>
       </c>
       <c r="X18" s="2">
         <v>0</v>
@@ -3268,8 +3261,8 @@
       <c r="R23" s="2">
         <v>0</v>
       </c>
-      <c r="S23" s="4">
-        <v>4</v>
+      <c r="S23" s="2">
+        <v>0</v>
       </c>
       <c r="T23" s="2">
         <v>0</v>
@@ -3893,8 +3886,8 @@
       <c r="M28" s="2">
         <v>0</v>
       </c>
-      <c r="N28" s="4">
-        <v>4</v>
+      <c r="N28" s="2">
+        <v>0</v>
       </c>
       <c r="O28" s="2">
         <v>0</v>
@@ -4649,8 +4642,8 @@
       <c r="I34" s="2">
         <v>0</v>
       </c>
-      <c r="J34" s="4">
-        <v>4</v>
+      <c r="J34" s="2">
+        <v>0</v>
       </c>
       <c r="K34" s="2">
         <v>0</v>

</xml_diff>